<commit_message>
working on seedlots workflow and wubi seed
</commit_message>
<xml_diff>
--- a/data/Cornell_WinterOatFounders_2024_Headrow_phenotypes.xlsx
+++ b/data/Cornell_WinterOatFounders_2024_Headrow_phenotypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2024_winter\2024_winter_intercrop\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2025_winter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780EA5DC-BDCA-4E7C-B364-074ADAE0E1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04261E3B-6A6E-4067-B0AA-F1A8A9F435C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2772" yWindow="17172" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1303,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>